<commit_message>
Add test for student_import with multiple students
</commit_message>
<xml_diff>
--- a/edziennik/tests/test_files/test_3students.xlsx
+++ b/edziennik/tests/test_files/test_3students.xlsx
@@ -212,14 +212,14 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>